<commit_message>
arquivo Concursos.xlsx atualizado: excluido a tabela inscrição
</commit_message>
<xml_diff>
--- a/Concursos.xlsx
+++ b/Concursos.xlsx
@@ -4,15 +4,14 @@
   <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Concurso" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Cargo" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Isncricao" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Avaliacao" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Conteudos" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Avaliacao" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Conteudos" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
   <extLst>
@@ -36,6 +35,12 @@
     <t>ano</t>
   </si>
   <si>
+    <t xml:space="preserve">inicio_inscrição (null)</t>
+  </si>
+  <si>
+    <t>fim_inscrição</t>
+  </si>
+  <si>
     <t>link</t>
   </si>
   <si>
@@ -51,6 +56,9 @@
     <t>nivel</t>
   </si>
   <si>
+    <t>taxa(null)</t>
+  </si>
+  <si>
     <t>c_reserva(null)</t>
   </si>
   <si>
@@ -72,34 +80,25 @@
     <t>Sim</t>
   </si>
   <si>
-    <t>data_inicial</t>
-  </si>
-  <si>
-    <t>data_final(null)</t>
-  </si>
-  <si>
-    <t>taxa(null)</t>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>carater</t>
+  </si>
+  <si>
+    <t>pontuacao</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>duracao</t>
+  </si>
+  <si>
+    <t>qtd_questoes</t>
   </si>
   <si>
     <t>id_cargo</t>
-  </si>
-  <si>
-    <t>tipo</t>
-  </si>
-  <si>
-    <t>carater</t>
-  </si>
-  <si>
-    <t>pontuacao</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>duracao</t>
-  </si>
-  <si>
-    <t>qtd_questoes</t>
   </si>
   <si>
     <t xml:space="preserve">Objetiva e Discursiva</t>
@@ -159,10 +158,10 @@
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="166" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -172,13 +171,23 @@
     <font>
       <b/>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="11.000000"/>
       <color indexed="65"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color indexed="2"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="0" tint="0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -215,7 +224,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -231,7 +240,17 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="3" applyNumberFormat="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="164" xfId="3" applyNumberFormat="1" applyFont="1" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
@@ -752,6 +771,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="9.1400000000000006"/>
     <col customWidth="1" min="3" max="3" style="0" width="14.65"/>
+    <col bestFit="1" min="5" max="5" width="19.57421875"/>
+    <col bestFit="1" min="6" max="6" width="14.421875"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15">
@@ -770,22 +791,34 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>2016</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
+      <c r="E2" s="4">
+        <v>42626</v>
+      </c>
+      <c r="F2" s="4">
+        <v>42646</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -803,19 +836,19 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" topLeftCell="A1" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" zoomScale="100" workbookViewId="0">
       <selection activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="9.1400000000000006"/>
     <col customWidth="1" min="2" max="2" style="0" width="23.289999999999999"/>
-    <col customWidth="1" min="3" max="3" style="0" width="14.57"/>
-    <col customWidth="1" min="4" max="4" style="0" width="14.51"/>
-    <col customWidth="1" min="5" max="5" style="1" width="9.8599999999999994"/>
-    <col customWidth="1" min="6" max="6" style="4" width="11.710000000000001"/>
-    <col customWidth="1" min="7" max="7" style="1" width="11.57"/>
+    <col customWidth="1" min="3" max="4" style="0" width="14.57"/>
+    <col customWidth="1" min="5" max="5" style="0" width="14.51"/>
+    <col customWidth="1" min="6" max="6" style="1" width="9.8599999999999994"/>
+    <col customWidth="1" min="7" max="7" style="5" width="11.710000000000001"/>
+    <col customWidth="1" min="8" max="8" style="1" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15">
@@ -826,19 +859,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" ht="15">
@@ -846,21 +882,24 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7">
+        <v>60</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1">
         <v>58</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="5">
         <v>5195.0900000000001</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>1</v>
       </c>
     </row>
@@ -879,69 +918,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" topLeftCell="A1" zoomScale="100" workbookViewId="0">
-      <selection activeCell="C8" activeCellId="0" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" style="1" width="9.1400000000000006"/>
-    <col customWidth="1" min="2" max="2" style="0" width="13.15"/>
-    <col customWidth="1" min="3" max="3" style="0" width="14.789999999999999"/>
-    <col customWidth="1" min="4" max="4" style="4" width="11"/>
-    <col customWidth="1" min="5" max="5" style="1" width="9.1400000000000006"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="5" customFormat="1" ht="15">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" ht="15">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>42626</v>
-      </c>
-      <c r="C2" s="6">
-        <v>42646</v>
-      </c>
-      <c r="D2" s="4">
-        <v>60</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="0" gridLines="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78750000000000009" bottom="0.78750000000000009" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr filterMode="0">
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" topLeftCell="A1" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" view="normal" zoomScale="100" workbookViewId="0">
       <selection activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -956,30 +933,30 @@
     <col customWidth="1" min="8" max="8" style="1" width="9.1400000000000006"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" ht="15">
+    <row r="1" s="8" customFormat="1" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" ht="15">
@@ -995,10 +972,10 @@
       <c r="D2" s="1">
         <v>120</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="9">
         <v>42722</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="10">
         <v>0.1875</v>
       </c>
       <c r="G2" s="1">
@@ -1016,7 +993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr filterMode="0">
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>

</xml_diff>

<commit_message>
concursos - criado a entidade conteudo com sucesso
</commit_message>
<xml_diff>
--- a/Concursos.xlsx
+++ b/Concursos.xlsx
@@ -4,7 +4,7 @@
   <workbookPr date1904="0"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório" sheetId="1" state="visible" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <t>carater</t>
   </si>
   <si>
-    <t>pontuacao</t>
+    <t>pontuacao(null)</t>
   </si>
   <si>
     <t>data</t>
@@ -95,7 +95,7 @@
     <t>duracao</t>
   </si>
   <si>
-    <t>qtd_questoes</t>
+    <t>qtd_questoes(null)</t>
   </si>
   <si>
     <t>id_cargo</t>
@@ -223,7 +223,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -254,6 +254,10 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1" applyProtection="0">
@@ -921,14 +925,14 @@
       <selection activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="9.1400000000000006"/>
     <col customWidth="1" min="2" max="2" style="0" width="22.289999999999999"/>
     <col customWidth="1" min="3" max="3" style="0" width="15.85"/>
-    <col customWidth="1" min="4" max="4" style="1" width="10.289999999999999"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="1" width="14.8515625"/>
     <col customWidth="1" min="5" max="5" style="0" width="12.710000000000001"/>
-    <col customWidth="1" min="7" max="7" style="1" width="13.289999999999999"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" style="1" width="17.421875"/>
     <col customWidth="1" min="8" max="8" style="1" width="9.1400000000000006"/>
   </cols>
   <sheetData>
@@ -968,16 +972,16 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="9">
         <v>120</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="10">
         <v>42722</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="11">
         <v>0.1875</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="9">
         <v>120</v>
       </c>
       <c r="H2" s="1">

</xml_diff>